<commit_message>
Add no matches array, change xlsx file template.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>juan</t>
+  </si>
+  <si>
+    <t>carlos</t>
+  </si>
+  <si>
+    <t>cz</t>
+  </si>
+  <si>
+    <t>esp</t>
+  </si>
+  <si>
+    <t>ben</t>
   </si>
 </sst>
 </file>
@@ -70,7 +82,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -102,8 +114,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
@@ -418,100 +442,128 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25" customFormat="1" s="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="6">
         <v>45</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="6">
         <v>68</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="6">
         <v>58</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="6">
         <v>30</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="6">
         <v>65</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>